<commit_message>
Added comments for BLAS routine.
</commit_message>
<xml_diff>
--- a/Perf Analysis.xlsx
+++ b/Perf Analysis.xlsx
@@ -4,23 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="606" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="in place transpose" sheetId="3" r:id="rId2"/>
+    <sheet name="IP transpose" sheetId="3" r:id="rId2"/>
     <sheet name="OPtranspose" sheetId="4" r:id="rId3"/>
-    <sheet name="basic in place compiler opt" sheetId="5" r:id="rId4"/>
+    <sheet name="basicIP compiler opt" sheetId="5" r:id="rId4"/>
     <sheet name="basic op compiler opt" sheetId="6" r:id="rId5"/>
+    <sheet name="Float IP" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'basic in place compiler opt'!$A$1:$L$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'in place transpose'!$A$1:$P$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'basic op compiler opt'!$A$1:$M$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'basicIP compiler opt'!$A$1:$L$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'IP transpose'!$A$1:$P$97</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">OPtranspose!$A$1:$P$61</definedName>
     <definedName name="better_output" localSheetId="0">'Memory Requirements'!$A$2:$B$7</definedName>
-    <definedName name="better_output2" localSheetId="1">'in place transpose'!$A$6:$O$81</definedName>
-    <definedName name="better_outputOn" localSheetId="3">'basic in place compiler opt'!$B$2:$L$21</definedName>
+    <definedName name="better_output2" localSheetId="1">'IP transpose'!$A$6:$O$81</definedName>
+    <definedName name="better_outputOn" localSheetId="3">'basicIP compiler opt'!$B$2:$L$21</definedName>
     <definedName name="better_outputop" localSheetId="2">OPtranspose!$B$2:$O$61</definedName>
+    <definedName name="ipbatch_caller2" localSheetId="5">'Float IP'!$A$2:$O$52</definedName>
     <definedName name="opbasic_batch_caller2" localSheetId="4">'basic op compiler opt'!$C$2:$L$21</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -102,7 +105,24 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="opbasic_batch_caller2.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="ipbatch_caller2.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:chandan:Developer:parallelprog2012:ipbatch_caller2.txt" tab="0" delimiter="|">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="opbasic_batch_caller2.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:chandan:Developer:parallelprog2012:opbasic_batch_caller2.txt" tab="0" delimiter="|">
       <textFields count="11">
         <textField/>
@@ -123,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="200">
   <si>
     <t>Matrix Size</t>
   </si>
@@ -558,6 +578,171 @@
   </si>
   <si>
     <t>Performance counter stats for './basictransposeOP3 -m 32768 -n 32768 -basic -noio -noinit' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -basic -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -basic -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -basic -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -1tiled -s1 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -1tiled -s1 8 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -1tiled -s1 16 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -1tiled -s1 32 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -1tiled -s1 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -1tiled -s1 8 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -1tiled -s1 16 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -1tiled -s1 32 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -1tiled -s1 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -1tiled -s1 8 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -1tiled -s1 16 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -1tiled -s1 32 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -2tiled -s1 4 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -2tiled -s1 8 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -2tiled -s1 8 -s2 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -2tiled -s1 16 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -2tiled -s1 16 -s2 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -2tiled -s1 16 -s2 8 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -2tiled -s1 32 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -2tiled -s1 32 -s2 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -2tiled -s1 32 -s2 8 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -2tiled -s1 32 -s2 16 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -2tiled -s1 4 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -2tiled -s1 8 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -2tiled -s1 8 -s2 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -2tiled -s1 16 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -2tiled -s1 16 -s2 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -2tiled -s1 16 -s2 8 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -2tiled -s1 32 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -2tiled -s1 32 -s2 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -2tiled -s1 32 -s2 8 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -2tiled -s1 32 -s2 16 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -2tiled -s1 4 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -2tiled -s1 8 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -2tiled -s1 8 -s2 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -2tiled -s1 16 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -2tiled -s1 16 -s2 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -2tiled -s1 16 -s2 8 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -2tiled -s1 32 -s2 2 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -2tiled -s1 32 -s2 4 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -2tiled -s1 32 -s2 8 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -2tiled -s1 32 -s2 16 -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -cacheob -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -cacheob -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -cacheob -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 8192 -mkl -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 16384 -mkl -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>Performance counter stats for './floattransposeIP -n 32768 -mkl -noio' (5 runs):</t>
+  </si>
+  <si>
+    <t>mkl</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Time(0.1s)</t>
+  </si>
+  <si>
+    <t>Ins/100Cycles</t>
   </si>
 </sst>
 </file>
@@ -654,7 +839,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -666,6 +851,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -844,7 +1041,7 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="9" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="10" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="177">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -926,6 +1123,12 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="9" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1008,6 +1211,12 @@
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="10" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1041,7 +1250,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'in place transpose'!$K$1</c:f>
+              <c:f>'IP transpose'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1052,7 +1261,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'in place transpose'!$D$2:$E$97</c:f>
+              <c:f>'IP transpose'!$D$2:$E$97</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -1142,7 +1351,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'in place transpose'!$K$2:$K$97</c:f>
+              <c:f>'IP transpose'!$K$2:$K$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1204,7 +1413,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'in place transpose'!$N$1</c:f>
+              <c:f>'IP transpose'!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1215,7 +1424,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'in place transpose'!$D$2:$E$97</c:f>
+              <c:f>'IP transpose'!$D$2:$E$97</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -1305,7 +1514,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'in place transpose'!$N$2:$N$97</c:f>
+              <c:f>'IP transpose'!$N$2:$N$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1367,7 +1576,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'in place transpose'!$P$1</c:f>
+              <c:f>'IP transpose'!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1378,7 +1587,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'in place transpose'!$D$2:$E$97</c:f>
+              <c:f>'IP transpose'!$D$2:$E$97</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -1468,7 +1677,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'in place transpose'!$P$2:$P$97</c:f>
+              <c:f>'IP transpose'!$P$2:$P$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1535,11 +1744,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="567192312"/>
-        <c:axId val="587347944"/>
+        <c:axId val="530334104"/>
+        <c:axId val="530337080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="567192312"/>
+        <c:axId val="530334104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1549,7 +1758,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587347944"/>
+        <c:crossAx val="530337080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1557,7 +1766,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="587347944"/>
+        <c:axId val="530337080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1568,7 +1777,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="567192312"/>
+        <c:crossAx val="530334104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1615,7 +1824,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'in place transpose'!$F$1</c:f>
+              <c:f>'IP transpose'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1626,7 +1835,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'in place transpose'!$D$2:$E$97</c:f>
+              <c:f>'IP transpose'!$D$2:$E$97</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -1716,7 +1925,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'in place transpose'!$F$2:$F$97</c:f>
+              <c:f>'IP transpose'!$F$2:$F$97</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1778,7 +1987,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'in place transpose'!$G$1</c:f>
+              <c:f>'IP transpose'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1789,7 +1998,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'in place transpose'!$D$2:$E$97</c:f>
+              <c:f>'IP transpose'!$D$2:$E$97</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="16"/>
                 <c:lvl>
@@ -1879,7 +2088,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'in place transpose'!$G$2:$G$97</c:f>
+              <c:f>'IP transpose'!$G$2:$G$97</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1946,11 +2155,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="568074392"/>
-        <c:axId val="611416264"/>
+        <c:axId val="510265656"/>
+        <c:axId val="529959720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="568074392"/>
+        <c:axId val="510265656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,7 +2168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="611416264"/>
+        <c:crossAx val="529959720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1967,7 +2176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="611416264"/>
+        <c:axId val="529959720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1978,7 +2187,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="568074392"/>
+        <c:crossAx val="510265656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2501,11 +2710,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="565971928"/>
-        <c:axId val="592327592"/>
+        <c:axId val="530399688"/>
+        <c:axId val="530402376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="565971928"/>
+        <c:axId val="530399688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2514,7 +2723,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592327592"/>
+        <c:crossAx val="530402376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2522,7 +2731,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="592327592"/>
+        <c:axId val="530402376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2533,7 +2742,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565971928"/>
+        <c:crossAx val="530399688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2580,7 +2789,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'basic in place compiler opt'!$C$1</c:f>
+              <c:f>'basicIP compiler opt'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2594,7 +2803,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'basic in place compiler opt'!$A$2:$B$21</c:f>
+              <c:f>'basicIP compiler opt'!$A$2:$B$21</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -2630,7 +2839,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'basic in place compiler opt'!$C$2:$C$21</c:f>
+              <c:f>'basicIP compiler opt'!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2656,7 +2865,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'basic in place compiler opt'!$D$1</c:f>
+              <c:f>'basicIP compiler opt'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2670,7 +2879,7 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'basic in place compiler opt'!$A$2:$B$21</c:f>
+              <c:f>'basicIP compiler opt'!$A$2:$B$21</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -2706,7 +2915,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'basic in place compiler opt'!$D$2:$D$21</c:f>
+              <c:f>'basicIP compiler opt'!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2737,11 +2946,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="537463208"/>
-        <c:axId val="537466184"/>
+        <c:axId val="530159656"/>
+        <c:axId val="530198232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="537463208"/>
+        <c:axId val="530159656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2750,7 +2959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="537466184"/>
+        <c:crossAx val="530198232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2758,7 +2967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="537466184"/>
+        <c:axId val="530198232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2769,7 +2978,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="537463208"/>
+        <c:crossAx val="530159656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2777,6 +2986,213 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'basic op compiler opt'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cycles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'basic op compiler opt'!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>O0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>O1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>O3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'basic op compiler opt'!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.29638900963E11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.25545799745E11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0458472023E11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.04716140521E11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'basic op compiler opt'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Instructions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'basic op compiler opt'!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>O0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>O1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>O3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'basic op compiler opt'!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.9517801793E10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2644371928E10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0823022604E10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.093530258E9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="530193240"/>
+        <c:axId val="530100472"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="530193240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="530100472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="530100472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="530193240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.755520341207349"/>
+          <c:y val="0.334531086839951"/>
+          <c:w val="0.222257436570429"/>
+          <c:h val="0.287927073631925"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2926,6 +3342,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1003300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="better_output" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -2943,7 +3394,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="opbasic_batch_caller2" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="opbasic_batch_caller2" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ipbatch_caller2" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3360,7 +3815,7 @@
   <dimension ref="A1:P97"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N105" sqref="N105"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3524,7 +3979,7 @@
         <v>2.0626780000000001E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P66" si="0">O3*10</f>
+        <f t="shared" ref="P3:P65" si="0">O3*10</f>
         <v>2.0626780000000001E-2</v>
       </c>
     </row>
@@ -6669,7 +7124,7 @@
         <v>2.3424611230000001</v>
       </c>
       <c r="P66">
-        <f>O66*10</f>
+        <f t="shared" ref="P66:P79" si="1">O66*10</f>
         <v>23.42461123</v>
       </c>
     </row>
@@ -6718,7 +7173,7 @@
         <v>1.639492516</v>
       </c>
       <c r="P67">
-        <f>O67*10</f>
+        <f t="shared" si="1"/>
         <v>16.39492516</v>
       </c>
     </row>
@@ -6767,7 +7222,7 @@
         <v>1.946363981</v>
       </c>
       <c r="P68">
-        <f>O68*10</f>
+        <f t="shared" si="1"/>
         <v>19.46363981</v>
       </c>
     </row>
@@ -6816,7 +7271,7 @@
         <v>2.5533310409999999</v>
       </c>
       <c r="P69">
-        <f>O69*10</f>
+        <f t="shared" si="1"/>
         <v>25.533310409999999</v>
       </c>
     </row>
@@ -6867,7 +7322,7 @@
         <v>3.1200618059999998</v>
       </c>
       <c r="P70">
-        <f>O70*10</f>
+        <f t="shared" si="1"/>
         <v>31.200618059999996</v>
       </c>
     </row>
@@ -6918,7 +7373,7 @@
         <v>2.5185371239999998</v>
       </c>
       <c r="P71">
-        <f>O71*10</f>
+        <f t="shared" si="1"/>
         <v>25.185371239999998</v>
       </c>
     </row>
@@ -6969,7 +7424,7 @@
         <v>1.8828633429999999</v>
       </c>
       <c r="P72">
-        <f>O72*10</f>
+        <f t="shared" si="1"/>
         <v>18.82863343</v>
       </c>
     </row>
@@ -7020,7 +7475,7 @@
         <v>2.2459805269999999</v>
       </c>
       <c r="P73">
-        <f>O73*10</f>
+        <f t="shared" si="1"/>
         <v>22.45980527</v>
       </c>
     </row>
@@ -7071,7 +7526,7 @@
         <v>1.70939095</v>
       </c>
       <c r="P74">
-        <f>O74*10</f>
+        <f t="shared" si="1"/>
         <v>17.093909499999999</v>
       </c>
     </row>
@@ -7122,7 +7577,7 @@
         <v>1.708017353</v>
       </c>
       <c r="P75">
-        <f>O75*10</f>
+        <f t="shared" si="1"/>
         <v>17.08017353</v>
       </c>
     </row>
@@ -7173,7 +7628,7 @@
         <v>1.883539386</v>
       </c>
       <c r="P76">
-        <f>O76*10</f>
+        <f t="shared" si="1"/>
         <v>18.83539386</v>
       </c>
     </row>
@@ -7224,7 +7679,7 @@
         <v>2.086529214</v>
       </c>
       <c r="P77">
-        <f>O77*10</f>
+        <f t="shared" si="1"/>
         <v>20.865292140000001</v>
       </c>
     </row>
@@ -7275,7 +7730,7 @@
         <v>1.5578961010000001</v>
       </c>
       <c r="P78">
-        <f>O78*10</f>
+        <f t="shared" si="1"/>
         <v>15.57896101</v>
       </c>
     </row>
@@ -7326,7 +7781,7 @@
         <v>1.5820253529999999</v>
       </c>
       <c r="P79">
-        <f>O79*10</f>
+        <f t="shared" si="1"/>
         <v>15.820253529999999</v>
       </c>
     </row>
@@ -7373,7 +7828,7 @@
         <v>3.5130777750000002</v>
       </c>
       <c r="P80">
-        <f t="shared" ref="P67:P97" si="1">O80*10</f>
+        <f t="shared" ref="P80:P97" si="2">O80*10</f>
         <v>35.13077775</v>
       </c>
     </row>
@@ -7420,7 +7875,7 @@
         <v>2.655187862</v>
       </c>
       <c r="P81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26.55187862</v>
       </c>
     </row>
@@ -7469,7 +7924,7 @@
         <v>8.9069770639999994</v>
       </c>
       <c r="P82">
-        <f>O82*10</f>
+        <f t="shared" ref="P82:P96" si="3">O82*10</f>
         <v>89.069770640000002</v>
       </c>
     </row>
@@ -7518,7 +7973,7 @@
         <v>6.6281234510000004</v>
       </c>
       <c r="P83">
-        <f>O83*10</f>
+        <f t="shared" si="3"/>
         <v>66.281234510000004</v>
       </c>
     </row>
@@ -7567,7 +8022,7 @@
         <v>8.190593818</v>
       </c>
       <c r="P84">
-        <f>O84*10</f>
+        <f t="shared" si="3"/>
         <v>81.905938179999993</v>
       </c>
     </row>
@@ -7616,7 +8071,7 @@
         <v>10.585622832</v>
       </c>
       <c r="P85">
-        <f>O85*10</f>
+        <f t="shared" si="3"/>
         <v>105.85622832</v>
       </c>
     </row>
@@ -7667,7 +8122,7 @@
         <v>12.639045058000001</v>
       </c>
       <c r="P86">
-        <f>O86*10</f>
+        <f t="shared" si="3"/>
         <v>126.39045058000001</v>
       </c>
     </row>
@@ -7718,7 +8173,7 @@
         <v>10.219585793</v>
       </c>
       <c r="P87">
-        <f>O87*10</f>
+        <f t="shared" si="3"/>
         <v>102.19585793</v>
       </c>
     </row>
@@ -7769,7 +8224,7 @@
         <v>7.5061385190000003</v>
       </c>
       <c r="P88">
-        <f>O88*10</f>
+        <f t="shared" si="3"/>
         <v>75.06138519000001</v>
       </c>
     </row>
@@ -7820,7 +8275,7 @@
         <v>9.0031480380000009</v>
       </c>
       <c r="P89">
-        <f>O89*10</f>
+        <f t="shared" si="3"/>
         <v>90.031480380000005</v>
       </c>
     </row>
@@ -7871,7 +8326,7 @@
         <v>6.8478988029999996</v>
       </c>
       <c r="P90">
-        <f>O90*10</f>
+        <f t="shared" si="3"/>
         <v>68.478988029999996</v>
       </c>
     </row>
@@ -7922,7 +8377,7 @@
         <v>6.8688592079999999</v>
       </c>
       <c r="P91">
-        <f>O91*10</f>
+        <f t="shared" si="3"/>
         <v>68.688592080000006</v>
       </c>
     </row>
@@ -7973,7 +8428,7 @@
         <v>7.8989883049999996</v>
       </c>
       <c r="P92">
-        <f>O92*10</f>
+        <f t="shared" si="3"/>
         <v>78.989883050000003</v>
       </c>
     </row>
@@ -8024,7 +8479,7 @@
         <v>8.4009302179999992</v>
       </c>
       <c r="P93">
-        <f>O93*10</f>
+        <f t="shared" si="3"/>
         <v>84.009302179999992</v>
       </c>
     </row>
@@ -8075,7 +8530,7 @@
         <v>6.317332296</v>
       </c>
       <c r="P94">
-        <f>O94*10</f>
+        <f t="shared" si="3"/>
         <v>63.17332296</v>
       </c>
     </row>
@@ -8126,7 +8581,7 @@
         <v>6.4657567680000003</v>
       </c>
       <c r="P95">
-        <f>O95*10</f>
+        <f t="shared" si="3"/>
         <v>64.65756768</v>
       </c>
     </row>
@@ -8175,7 +8630,7 @@
         <v>20.095424079000001</v>
       </c>
       <c r="P96">
-        <f>O96*10</f>
+        <f t="shared" si="3"/>
         <v>200.95424079</v>
       </c>
     </row>
@@ -8224,7 +8679,7 @@
         <v>11.711669229</v>
       </c>
       <c r="P97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>117.11669229</v>
       </c>
     </row>
@@ -8256,7 +8711,7 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8362,7 +8817,7 @@
         <v>107.84</v>
       </c>
       <c r="N2">
-        <f>O2*10</f>
+        <f t="shared" ref="N2:N33" si="0">O2*10</f>
         <v>2.9485420600000003</v>
       </c>
       <c r="O2">
@@ -8409,7 +8864,7 @@
         <v>113.04</v>
       </c>
       <c r="N3">
-        <f>O3*10</f>
+        <f t="shared" si="0"/>
         <v>14.520867630000001</v>
       </c>
       <c r="O3">
@@ -8456,7 +8911,7 @@
         <v>114.38</v>
       </c>
       <c r="N4">
-        <f>O4*10</f>
+        <f t="shared" si="0"/>
         <v>54.846424049999996</v>
       </c>
       <c r="O4">
@@ -8505,7 +8960,7 @@
         <v>113.85</v>
       </c>
       <c r="N5">
-        <f>O5*10</f>
+        <f t="shared" si="0"/>
         <v>326.18692447999996</v>
       </c>
       <c r="O5">
@@ -8554,7 +9009,7 @@
         <v>38.159999999999997</v>
       </c>
       <c r="N6">
-        <f>O6*10</f>
+        <f t="shared" si="0"/>
         <v>1.1710600499999999</v>
       </c>
       <c r="O6">
@@ -8603,7 +9058,7 @@
         <v>39.08</v>
       </c>
       <c r="N7">
-        <f>O7*10</f>
+        <f t="shared" si="0"/>
         <v>0.99753882000000005</v>
       </c>
       <c r="O7">
@@ -8652,7 +9107,7 @@
         <v>93.53</v>
       </c>
       <c r="N8">
-        <f>O8*10</f>
+        <f t="shared" si="0"/>
         <v>1.28663894</v>
       </c>
       <c r="O8">
@@ -8701,7 +9156,7 @@
         <v>111.5</v>
       </c>
       <c r="N9">
-        <f>O9*10</f>
+        <f t="shared" si="0"/>
         <v>1.4886210099999999</v>
       </c>
       <c r="O9">
@@ -8750,7 +9205,7 @@
         <v>39.61</v>
       </c>
       <c r="N10">
-        <f>O10*10</f>
+        <f t="shared" si="0"/>
         <v>5.22319479</v>
       </c>
       <c r="O10">
@@ -8799,7 +9254,7 @@
         <v>41.06</v>
       </c>
       <c r="N11">
-        <f>O11*10</f>
+        <f t="shared" si="0"/>
         <v>4.1645597199999997</v>
       </c>
       <c r="O11">
@@ -8848,7 +9303,7 @@
         <v>91.9</v>
       </c>
       <c r="N12">
-        <f>O12*10</f>
+        <f t="shared" si="0"/>
         <v>6.1633158400000001</v>
       </c>
       <c r="O12">
@@ -8897,7 +9352,7 @@
         <v>117.32</v>
       </c>
       <c r="N13">
-        <f>O13*10</f>
+        <f t="shared" si="0"/>
         <v>5.7937417</v>
       </c>
       <c r="O13">
@@ -8946,7 +9401,7 @@
         <v>40.04</v>
       </c>
       <c r="N14">
-        <f>O14*10</f>
+        <f t="shared" si="0"/>
         <v>20.457833449999999</v>
       </c>
       <c r="O14">
@@ -8995,7 +9450,7 @@
         <v>41.53</v>
       </c>
       <c r="N15">
-        <f>O15*10</f>
+        <f t="shared" si="0"/>
         <v>16.722930680000001</v>
       </c>
       <c r="O15">
@@ -9044,7 +9499,7 @@
         <v>96.44</v>
       </c>
       <c r="N16">
-        <f>O16*10</f>
+        <f t="shared" si="0"/>
         <v>26.02246762</v>
       </c>
       <c r="O16">
@@ -9093,7 +9548,7 @@
         <v>117.92</v>
       </c>
       <c r="N17">
-        <f>O17*10</f>
+        <f t="shared" si="0"/>
         <v>23.25319279</v>
       </c>
       <c r="O17">
@@ -9142,7 +9597,7 @@
         <v>40.17</v>
       </c>
       <c r="N18">
-        <f>O18*10</f>
+        <f t="shared" si="0"/>
         <v>99.865478469999999</v>
       </c>
       <c r="O18">
@@ -9191,7 +9646,7 @@
         <v>41.7</v>
       </c>
       <c r="N19">
-        <f>O19*10</f>
+        <f t="shared" si="0"/>
         <v>72.025963050000001</v>
       </c>
       <c r="O19">
@@ -9240,7 +9695,7 @@
         <v>99.49</v>
       </c>
       <c r="N20">
-        <f>O20*10</f>
+        <f t="shared" si="0"/>
         <v>116.89149350999999</v>
       </c>
       <c r="O20">
@@ -9289,7 +9744,7 @@
         <v>118.06</v>
       </c>
       <c r="N21">
-        <f>O21*10</f>
+        <f t="shared" si="0"/>
         <v>108.17246485</v>
       </c>
       <c r="O21">
@@ -9340,7 +9795,7 @@
         <v>15.97</v>
       </c>
       <c r="N22">
-        <f>O22*10</f>
+        <f t="shared" si="0"/>
         <v>1.47144641</v>
       </c>
       <c r="O22">
@@ -9391,7 +9846,7 @@
         <v>18.32</v>
       </c>
       <c r="N23">
-        <f>O23*10</f>
+        <f t="shared" si="0"/>
         <v>1.26126702</v>
       </c>
       <c r="O23">
@@ -9442,7 +9897,7 @@
         <v>27.93</v>
       </c>
       <c r="N24">
-        <f>O24*10</f>
+        <f t="shared" si="0"/>
         <v>1.03315983</v>
       </c>
       <c r="O24">
@@ -9493,7 +9948,7 @@
         <v>35.979999999999997</v>
       </c>
       <c r="N25">
-        <f>O25*10</f>
+        <f t="shared" si="0"/>
         <v>1.3956436800000001</v>
       </c>
       <c r="O25">
@@ -9544,7 +9999,7 @@
         <v>38.92</v>
       </c>
       <c r="N26">
-        <f>O26*10</f>
+        <f t="shared" si="0"/>
         <v>0.97389658000000001</v>
       </c>
       <c r="O26">
@@ -9595,7 +10050,7 @@
         <v>46.4</v>
       </c>
       <c r="N27">
-        <f>O27*10</f>
+        <f t="shared" si="0"/>
         <v>0.94051953999999993</v>
       </c>
       <c r="O27">
@@ -9646,7 +10101,7 @@
         <v>36</v>
       </c>
       <c r="N28">
-        <f>O28*10</f>
+        <f t="shared" si="0"/>
         <v>1.46126055</v>
       </c>
       <c r="O28">
@@ -9697,7 +10152,7 @@
         <v>39.76</v>
       </c>
       <c r="N29">
-        <f>O29*10</f>
+        <f t="shared" si="0"/>
         <v>0.99282121000000001</v>
       </c>
       <c r="O29">
@@ -9748,7 +10203,7 @@
         <v>48.3</v>
       </c>
       <c r="N30">
-        <f>O30*10</f>
+        <f t="shared" si="0"/>
         <v>0.96840285999999998</v>
       </c>
       <c r="O30">
@@ -9799,7 +10254,7 @@
         <v>94.43</v>
       </c>
       <c r="N31">
-        <f>O31*10</f>
+        <f t="shared" si="0"/>
         <v>1.25537861</v>
       </c>
       <c r="O31">
@@ -9850,7 +10305,7 @@
         <v>16.2</v>
       </c>
       <c r="N32">
-        <f>O32*10</f>
+        <f t="shared" si="0"/>
         <v>5.6070313000000009</v>
       </c>
       <c r="O32">
@@ -9901,7 +10356,7 @@
         <v>18.600000000000001</v>
       </c>
       <c r="N33">
-        <f>O33*10</f>
+        <f t="shared" si="0"/>
         <v>4.8249112900000002</v>
       </c>
       <c r="O33">
@@ -9952,7 +10407,7 @@
         <v>28.82</v>
       </c>
       <c r="N34">
-        <f>O34*10</f>
+        <f t="shared" ref="N34:N65" si="1">O34*10</f>
         <v>4.2119513800000004</v>
       </c>
       <c r="O34">
@@ -10003,7 +10458,7 @@
         <v>36.18</v>
       </c>
       <c r="N35">
-        <f>O35*10</f>
+        <f t="shared" si="1"/>
         <v>5.93566225</v>
       </c>
       <c r="O35">
@@ -10054,7 +10509,7 @@
         <v>39.67</v>
       </c>
       <c r="N36">
-        <f>O36*10</f>
+        <f t="shared" si="1"/>
         <v>4.1284101099999999</v>
       </c>
       <c r="O36">
@@ -10105,7 +10560,7 @@
         <v>47.93</v>
       </c>
       <c r="N37">
-        <f>O37*10</f>
+        <f t="shared" si="1"/>
         <v>3.9135844800000004</v>
       </c>
       <c r="O37">
@@ -10156,7 +10611,7 @@
         <v>36.93</v>
       </c>
       <c r="N38">
-        <f>O38*10</f>
+        <f t="shared" si="1"/>
         <v>5.5778085300000004</v>
       </c>
       <c r="O38">
@@ -10207,7 +10662,7 @@
         <v>41.26</v>
       </c>
       <c r="N39">
-        <f>O39*10</f>
+        <f t="shared" si="1"/>
         <v>4.0565192999999997</v>
       </c>
       <c r="O39">
@@ -10258,7 +10713,7 @@
         <v>49.52</v>
       </c>
       <c r="N40">
-        <f>O40*10</f>
+        <f t="shared" si="1"/>
         <v>3.9230348500000001</v>
       </c>
       <c r="O40">
@@ -10309,7 +10764,7 @@
         <v>93.82</v>
       </c>
       <c r="N41">
-        <f>O41*10</f>
+        <f t="shared" si="1"/>
         <v>6.1433102699999997</v>
       </c>
       <c r="O41">
@@ -10360,7 +10815,7 @@
         <v>16.27</v>
       </c>
       <c r="N42">
-        <f>O42*10</f>
+        <f t="shared" si="1"/>
         <v>23.5061134</v>
       </c>
       <c r="O42">
@@ -10411,7 +10866,7 @@
         <v>18.84</v>
       </c>
       <c r="N43">
-        <f>O43*10</f>
+        <f t="shared" si="1"/>
         <v>20.002439089999999</v>
       </c>
       <c r="O43">
@@ -10462,7 +10917,7 @@
         <v>28.99</v>
       </c>
       <c r="N44">
-        <f>O44*10</f>
+        <f t="shared" si="1"/>
         <v>16.90975444</v>
       </c>
       <c r="O44">
@@ -10513,7 +10968,7 @@
         <v>36.21</v>
       </c>
       <c r="N45">
-        <f>O45*10</f>
+        <f t="shared" si="1"/>
         <v>24.237200170000001</v>
       </c>
       <c r="O45">
@@ -10564,7 +11019,7 @@
         <v>40.01</v>
       </c>
       <c r="N46">
-        <f>O46*10</f>
+        <f t="shared" si="1"/>
         <v>16.886211920000001</v>
       </c>
       <c r="O46">
@@ -10615,7 +11070,7 @@
         <v>47.71</v>
       </c>
       <c r="N47">
-        <f>O47*10</f>
+        <f t="shared" si="1"/>
         <v>15.779938849999999</v>
       </c>
       <c r="O47">
@@ -10666,7 +11121,7 @@
         <v>36.92</v>
       </c>
       <c r="N48">
-        <f>O48*10</f>
+        <f t="shared" si="1"/>
         <v>22.639294529999997</v>
       </c>
       <c r="O48">
@@ -10717,7 +11172,7 @@
         <v>41.25</v>
       </c>
       <c r="N49">
-        <f>O49*10</f>
+        <f t="shared" si="1"/>
         <v>16.453128640000003</v>
       </c>
       <c r="O49">
@@ -10768,7 +11223,7 @@
         <v>49.62</v>
       </c>
       <c r="N50">
-        <f>O50*10</f>
+        <f t="shared" si="1"/>
         <v>15.907551250000001</v>
       </c>
       <c r="O50">
@@ -10819,7 +11274,7 @@
         <v>97.3</v>
       </c>
       <c r="N51">
-        <f>O51*10</f>
+        <f t="shared" si="1"/>
         <v>25.66024771</v>
       </c>
       <c r="O51">
@@ -10870,7 +11325,7 @@
         <v>16.309999999999999</v>
       </c>
       <c r="N52">
-        <f>O52*10</f>
+        <f t="shared" si="1"/>
         <v>108.37322178999999</v>
       </c>
       <c r="O52">
@@ -10921,7 +11376,7 @@
         <v>18.97</v>
       </c>
       <c r="N53">
-        <f>O53*10</f>
+        <f t="shared" si="1"/>
         <v>82.716646690000005</v>
       </c>
       <c r="O53">
@@ -10972,7 +11427,7 @@
         <v>29.04</v>
       </c>
       <c r="N54">
-        <f>O54*10</f>
+        <f t="shared" si="1"/>
         <v>71.613150210000001</v>
       </c>
       <c r="O54">
@@ -11023,7 +11478,7 @@
         <v>36.49</v>
       </c>
       <c r="N55">
-        <f>O55*10</f>
+        <f t="shared" si="1"/>
         <v>108.99784707000001</v>
       </c>
       <c r="O55">
@@ -11074,7 +11529,7 @@
         <v>39.950000000000003</v>
       </c>
       <c r="N56">
-        <f>O56*10</f>
+        <f t="shared" si="1"/>
         <v>74.385422930000004</v>
       </c>
       <c r="O56">
@@ -11125,7 +11580,7 @@
         <v>47.81</v>
       </c>
       <c r="N57">
-        <f>O57*10</f>
+        <f t="shared" si="1"/>
         <v>66.781835220000005</v>
       </c>
       <c r="O57">
@@ -11176,7 +11631,7 @@
         <v>36.93</v>
       </c>
       <c r="N58">
-        <f>O58*10</f>
+        <f t="shared" si="1"/>
         <v>101.91932908</v>
       </c>
       <c r="O58">
@@ -11227,7 +11682,7 @@
         <v>41.18</v>
       </c>
       <c r="N59">
-        <f>O59*10</f>
+        <f t="shared" si="1"/>
         <v>73.541192899999999</v>
       </c>
       <c r="O59">
@@ -11278,7 +11733,7 @@
         <v>49.41</v>
       </c>
       <c r="N60">
-        <f>O60*10</f>
+        <f t="shared" si="1"/>
         <v>66.525458669999992</v>
       </c>
       <c r="O60">
@@ -11329,7 +11784,7 @@
         <v>98.87</v>
       </c>
       <c r="N61">
-        <f>O61*10</f>
+        <f t="shared" si="1"/>
         <v>113.98480206000001</v>
       </c>
       <c r="O61">
@@ -12205,10 +12660,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12264,7 +12720,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" hidden="1">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -12305,7 +12761,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" hidden="1">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -12346,7 +12802,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" hidden="1">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -12387,7 +12843,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" hidden="1">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -12428,7 +12884,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" hidden="1">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -12469,7 +12925,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" hidden="1">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -12510,7 +12966,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" hidden="1">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -12551,7 +13007,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" hidden="1">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -12592,7 +13048,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" hidden="1">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -12633,7 +13089,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" hidden="1">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -12674,7 +13130,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" hidden="1">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -12715,7 +13171,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" hidden="1">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -12756,7 +13212,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" hidden="1">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -12797,7 +13253,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" hidden="1">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -12838,7 +13294,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" hidden="1">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -12879,7 +13335,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" hidden="1">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -13085,9 +13541,2819 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M21">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="32768"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:M21">
     <sortCondition ref="B5"/>
   </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.1640625" customWidth="1"/>
+    <col min="18" max="18" width="77.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2">
+        <v>8192</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2824325269</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1596074001</v>
+      </c>
+      <c r="G2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H2">
+        <f>G2*100</f>
+        <v>56.999999999999993</v>
+      </c>
+      <c r="I2" s="1">
+        <v>40684884</v>
+      </c>
+      <c r="J2" s="1">
+        <v>39642196</v>
+      </c>
+      <c r="K2">
+        <v>97.436999999999998</v>
+      </c>
+      <c r="L2" s="1">
+        <v>71944463</v>
+      </c>
+      <c r="M2" s="1">
+        <v>46476578</v>
+      </c>
+      <c r="N2">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="O2">
+        <v>0.85473194799999996</v>
+      </c>
+      <c r="P2">
+        <f>O2*10</f>
+        <v>8.5473194799999987</v>
+      </c>
+      <c r="R2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3">
+        <v>16384</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="1">
+        <v>11197061043</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6376130308</v>
+      </c>
+      <c r="G3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H52" si="0">G3*100</f>
+        <v>56.999999999999993</v>
+      </c>
+      <c r="I3" s="1">
+        <v>166238681</v>
+      </c>
+      <c r="J3" s="1">
+        <v>159295005</v>
+      </c>
+      <c r="K3">
+        <v>95.822999999999993</v>
+      </c>
+      <c r="L3" s="1">
+        <v>284015890</v>
+      </c>
+      <c r="M3" s="1">
+        <v>190358849</v>
+      </c>
+      <c r="N3">
+        <v>67.02</v>
+      </c>
+      <c r="O3">
+        <v>3.3852986239999998</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P52" si="1">O3*10</f>
+        <v>33.85298624</v>
+      </c>
+      <c r="R3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4">
+        <v>32768</v>
+      </c>
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="1">
+        <v>57893454162</v>
+      </c>
+      <c r="F4" s="1">
+        <v>25498240980</v>
+      </c>
+      <c r="G4">
+        <v>0.44</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="I4" s="1">
+        <v>691508760</v>
+      </c>
+      <c r="J4" s="1">
+        <v>638177946</v>
+      </c>
+      <c r="K4">
+        <v>92.287999999999997</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1138060680</v>
+      </c>
+      <c r="M4" s="1">
+        <v>800348472</v>
+      </c>
+      <c r="N4">
+        <v>70.33</v>
+      </c>
+      <c r="O4">
+        <v>17.502657431999999</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>175.02657432000001</v>
+      </c>
+      <c r="R4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5">
+        <v>8192</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1905568909</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2371895252</v>
+      </c>
+      <c r="G5">
+        <v>1.24</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="I5" s="1">
+        <v>23361380</v>
+      </c>
+      <c r="J5" s="1">
+        <v>22848265</v>
+      </c>
+      <c r="K5">
+        <v>97.804000000000002</v>
+      </c>
+      <c r="L5" s="1">
+        <v>136709466</v>
+      </c>
+      <c r="M5" s="1">
+        <v>28185538</v>
+      </c>
+      <c r="N5">
+        <v>20.62</v>
+      </c>
+      <c r="O5">
+        <v>0.57727105099999998</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>5.7727105099999996</v>
+      </c>
+      <c r="R5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6">
+        <v>8192</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1461905629</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1986377393</v>
+      </c>
+      <c r="G6">
+        <v>1.36</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="I6" s="1">
+        <v>16098403</v>
+      </c>
+      <c r="J6" s="1">
+        <v>15243243</v>
+      </c>
+      <c r="K6">
+        <v>94.688000000000002</v>
+      </c>
+      <c r="L6" s="1">
+        <v>102676965</v>
+      </c>
+      <c r="M6" s="1">
+        <v>23827486</v>
+      </c>
+      <c r="N6">
+        <v>23.21</v>
+      </c>
+      <c r="O6">
+        <v>0.44327536299999998</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>4.4327536299999997</v>
+      </c>
+      <c r="R6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7">
+        <v>8192</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1653125458</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1814545804</v>
+      </c>
+      <c r="G7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="I7" s="1">
+        <v>37465249</v>
+      </c>
+      <c r="J7" s="1">
+        <v>12076173</v>
+      </c>
+      <c r="K7">
+        <v>32.232999999999997</v>
+      </c>
+      <c r="L7" s="1">
+        <v>92990214</v>
+      </c>
+      <c r="M7" s="1">
+        <v>54469532</v>
+      </c>
+      <c r="N7">
+        <v>58.58</v>
+      </c>
+      <c r="O7">
+        <v>0.50093148799999998</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>5.0093148799999998</v>
+      </c>
+      <c r="R7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8">
+        <v>8192</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2163631388</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1738418830</v>
+      </c>
+      <c r="G8">
+        <v>0.8</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="I8" s="1">
+        <v>63208072</v>
+      </c>
+      <c r="J8" s="1">
+        <v>10253851</v>
+      </c>
+      <c r="K8">
+        <v>16.222000000000001</v>
+      </c>
+      <c r="L8" s="1">
+        <v>89985885</v>
+      </c>
+      <c r="M8" s="1">
+        <v>71772368</v>
+      </c>
+      <c r="N8">
+        <v>79.760000000000005</v>
+      </c>
+      <c r="O8">
+        <v>0.65509818399999997</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>6.5509818399999995</v>
+      </c>
+      <c r="R8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9">
+        <v>16384</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7524045723</v>
+      </c>
+      <c r="F9" s="1">
+        <v>9473929202</v>
+      </c>
+      <c r="G9">
+        <v>1.26</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="I9" s="1">
+        <v>87250143</v>
+      </c>
+      <c r="J9" s="1">
+        <v>85716358</v>
+      </c>
+      <c r="K9">
+        <v>98.242000000000004</v>
+      </c>
+      <c r="L9" s="1">
+        <v>543001112</v>
+      </c>
+      <c r="M9" s="1">
+        <v>106497272</v>
+      </c>
+      <c r="N9">
+        <v>19.61</v>
+      </c>
+      <c r="O9">
+        <v>2.2759842830000001</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>22.75984283</v>
+      </c>
+      <c r="R9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10">
+        <v>16384</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5824324058</v>
+      </c>
+      <c r="F10" s="1">
+        <v>7941831023</v>
+      </c>
+      <c r="G10">
+        <v>1.36</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="I10" s="1">
+        <v>63465865</v>
+      </c>
+      <c r="J10" s="1">
+        <v>60398238</v>
+      </c>
+      <c r="K10">
+        <v>95.165999999999997</v>
+      </c>
+      <c r="L10" s="1">
+        <v>406096079</v>
+      </c>
+      <c r="M10" s="1">
+        <v>94177416</v>
+      </c>
+      <c r="N10">
+        <v>23.19</v>
+      </c>
+      <c r="O10">
+        <v>1.762619106</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>17.62619106</v>
+      </c>
+      <c r="R10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11">
+        <v>16384</v>
+      </c>
+      <c r="B11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1">
+        <v>6634232635</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7261145381</v>
+      </c>
+      <c r="G11">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>109.00000000000001</v>
+      </c>
+      <c r="I11" s="1">
+        <v>150105348</v>
+      </c>
+      <c r="J11" s="1">
+        <v>48380524</v>
+      </c>
+      <c r="K11">
+        <v>32.231000000000002</v>
+      </c>
+      <c r="L11" s="1">
+        <v>368431200</v>
+      </c>
+      <c r="M11" s="1">
+        <v>217523853</v>
+      </c>
+      <c r="N11">
+        <v>59.04</v>
+      </c>
+      <c r="O11">
+        <v>2.0066723450000001</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>20.066723450000001</v>
+      </c>
+      <c r="R11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12">
+        <v>16384</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8635272853</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6941859364</v>
+      </c>
+      <c r="G12">
+        <v>0.8</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="I12" s="1">
+        <v>253205952</v>
+      </c>
+      <c r="J12" s="1">
+        <v>41052471</v>
+      </c>
+      <c r="K12">
+        <v>16.213000000000001</v>
+      </c>
+      <c r="L12" s="1">
+        <v>357123027</v>
+      </c>
+      <c r="M12" s="1">
+        <v>286538290</v>
+      </c>
+      <c r="N12">
+        <v>80.239999999999995</v>
+      </c>
+      <c r="O12">
+        <v>2.6105311200000001</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>26.105311200000003</v>
+      </c>
+      <c r="R12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13">
+        <v>32768</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>30119741604</v>
+      </c>
+      <c r="F13" s="1">
+        <v>37885570883</v>
+      </c>
+      <c r="G13">
+        <v>1.26</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="I13" s="1">
+        <v>350164310</v>
+      </c>
+      <c r="J13" s="1">
+        <v>343454875</v>
+      </c>
+      <c r="K13">
+        <v>98.084000000000003</v>
+      </c>
+      <c r="L13" s="1">
+        <v>2168719672</v>
+      </c>
+      <c r="M13" s="1">
+        <v>427451256</v>
+      </c>
+      <c r="N13">
+        <v>19.71</v>
+      </c>
+      <c r="O13">
+        <v>9.1088452689999997</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>91.088452689999997</v>
+      </c>
+      <c r="R13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14">
+        <v>32768</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1">
+        <v>23567640713</v>
+      </c>
+      <c r="F14" s="1">
+        <v>31753450211</v>
+      </c>
+      <c r="G14">
+        <v>1.35</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="I14" s="1">
+        <v>253815875</v>
+      </c>
+      <c r="J14" s="1">
+        <v>240932722</v>
+      </c>
+      <c r="K14">
+        <v>94.924000000000007</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1621599066</v>
+      </c>
+      <c r="M14" s="1">
+        <v>374363709</v>
+      </c>
+      <c r="N14">
+        <v>23.09</v>
+      </c>
+      <c r="O14">
+        <v>7.128484662</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
+        <v>71.284846619999996</v>
+      </c>
+      <c r="R14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15">
+        <v>32768</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1">
+        <v>28052269361</v>
+      </c>
+      <c r="F15" s="1">
+        <v>29037234190</v>
+      </c>
+      <c r="G15">
+        <v>1.04</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="I15" s="1">
+        <v>614327613</v>
+      </c>
+      <c r="J15" s="1">
+        <v>190802671</v>
+      </c>
+      <c r="K15">
+        <v>31.059000000000001</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1469479170</v>
+      </c>
+      <c r="M15" s="1">
+        <v>898201854</v>
+      </c>
+      <c r="N15">
+        <v>61.12</v>
+      </c>
+      <c r="O15">
+        <v>8.4879221250000008</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
+        <v>84.879221250000001</v>
+      </c>
+      <c r="R15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16">
+        <v>32768</v>
+      </c>
+      <c r="B16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1">
+        <v>36017508760</v>
+      </c>
+      <c r="F16" s="1">
+        <v>27772581575</v>
+      </c>
+      <c r="G16">
+        <v>0.77</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1272393633</v>
+      </c>
+      <c r="J16" s="1">
+        <v>157022463</v>
+      </c>
+      <c r="K16">
+        <v>12.340999999999999</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1425685092</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1429386240</v>
+      </c>
+      <c r="N16">
+        <v>100.26</v>
+      </c>
+      <c r="O16">
+        <v>10.891838106</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="1"/>
+        <v>108.91838106</v>
+      </c>
+      <c r="R16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17">
+        <v>8192</v>
+      </c>
+      <c r="B17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2672150901</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3682899423</v>
+      </c>
+      <c r="G17">
+        <v>1.38</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="I17" s="1">
+        <v>19217771</v>
+      </c>
+      <c r="J17" s="1">
+        <v>18840772</v>
+      </c>
+      <c r="K17">
+        <v>98.037999999999997</v>
+      </c>
+      <c r="L17" s="1">
+        <v>348598274</v>
+      </c>
+      <c r="M17" s="1">
+        <v>23781172</v>
+      </c>
+      <c r="N17">
+        <v>6.82</v>
+      </c>
+      <c r="O17">
+        <v>0.80856055500000001</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="1"/>
+        <v>8.0856055500000004</v>
+      </c>
+      <c r="R17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18">
+        <v>8192</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2099171957</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3450975432</v>
+      </c>
+      <c r="G18">
+        <v>1.64</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="I18" s="1">
+        <v>16247946</v>
+      </c>
+      <c r="J18" s="1">
+        <v>15530788</v>
+      </c>
+      <c r="K18">
+        <v>95.585999999999999</v>
+      </c>
+      <c r="L18" s="1">
+        <v>328436987</v>
+      </c>
+      <c r="M18" s="1">
+        <v>23383327</v>
+      </c>
+      <c r="N18">
+        <v>7.12</v>
+      </c>
+      <c r="O18">
+        <v>0.63549517799999999</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="1"/>
+        <v>6.3549517800000004</v>
+      </c>
+      <c r="R18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19">
+        <v>8192</v>
+      </c>
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1558310962</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2493570342</v>
+      </c>
+      <c r="G19">
+        <v>1.6</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="I19" s="1">
+        <v>15928524</v>
+      </c>
+      <c r="J19" s="1">
+        <v>15035535</v>
+      </c>
+      <c r="K19">
+        <v>94.394000000000005</v>
+      </c>
+      <c r="L19" s="1">
+        <v>155513498</v>
+      </c>
+      <c r="M19" s="1">
+        <v>23175104</v>
+      </c>
+      <c r="N19">
+        <v>14.9</v>
+      </c>
+      <c r="O19">
+        <v>0.472484705</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="1"/>
+        <v>4.7248470500000002</v>
+      </c>
+      <c r="R19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20">
+        <v>8192</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1921253124</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3371153815</v>
+      </c>
+      <c r="G20">
+        <v>1.75</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="I20" s="1">
+        <v>35419323</v>
+      </c>
+      <c r="J20" s="1">
+        <v>12358444</v>
+      </c>
+      <c r="K20">
+        <v>34.892000000000003</v>
+      </c>
+      <c r="L20" s="1">
+        <v>327041216</v>
+      </c>
+      <c r="M20" s="1">
+        <v>48087115</v>
+      </c>
+      <c r="N20">
+        <v>14.7</v>
+      </c>
+      <c r="O20">
+        <v>0.58586286300000001</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="1"/>
+        <v>5.8586286300000001</v>
+      </c>
+      <c r="R20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21">
+        <v>8192</v>
+      </c>
+      <c r="B21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1451925331</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2448974353</v>
+      </c>
+      <c r="G21">
+        <v>1.69</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>169</v>
+      </c>
+      <c r="I21" s="1">
+        <v>29677040</v>
+      </c>
+      <c r="J21" s="1">
+        <v>12332574</v>
+      </c>
+      <c r="K21">
+        <v>41.555999999999997</v>
+      </c>
+      <c r="L21" s="1">
+        <v>151302927</v>
+      </c>
+      <c r="M21" s="1">
+        <v>40371591</v>
+      </c>
+      <c r="N21">
+        <v>26.68</v>
+      </c>
+      <c r="O21">
+        <v>0.440635153</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="1"/>
+        <v>4.4063515300000002</v>
+      </c>
+      <c r="R21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22">
+        <v>8192</v>
+      </c>
+      <c r="B22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1478346692</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2040122834</v>
+      </c>
+      <c r="G22">
+        <v>1.38</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="I22" s="1">
+        <v>30870479</v>
+      </c>
+      <c r="J22" s="1">
+        <v>12557925</v>
+      </c>
+      <c r="K22">
+        <v>40.679000000000002</v>
+      </c>
+      <c r="L22" s="1">
+        <v>112503458</v>
+      </c>
+      <c r="M22" s="1">
+        <v>42179862</v>
+      </c>
+      <c r="N22">
+        <v>37.49</v>
+      </c>
+      <c r="O22">
+        <v>0.448709949</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="1"/>
+        <v>4.4870994900000003</v>
+      </c>
+      <c r="R22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23">
+        <v>8192</v>
+      </c>
+      <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23">
+        <v>32</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1768891971</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3343998936</v>
+      </c>
+      <c r="G23">
+        <v>1.89</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>189</v>
+      </c>
+      <c r="I23" s="1">
+        <v>44206538</v>
+      </c>
+      <c r="J23" s="1">
+        <v>10289981</v>
+      </c>
+      <c r="K23">
+        <v>23.277000000000001</v>
+      </c>
+      <c r="L23" s="1">
+        <v>328358290</v>
+      </c>
+      <c r="M23" s="1">
+        <v>53791128</v>
+      </c>
+      <c r="N23">
+        <v>16.38</v>
+      </c>
+      <c r="O23">
+        <v>0.53603023900000002</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="1"/>
+        <v>5.3603023900000002</v>
+      </c>
+      <c r="R23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24">
+        <v>8192</v>
+      </c>
+      <c r="B24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1351840105</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2440191636</v>
+      </c>
+      <c r="G24">
+        <v>1.81</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+      <c r="I24" s="1">
+        <v>31705361</v>
+      </c>
+      <c r="J24" s="1">
+        <v>10471934</v>
+      </c>
+      <c r="K24">
+        <v>33.029000000000003</v>
+      </c>
+      <c r="L24" s="1">
+        <v>151429831</v>
+      </c>
+      <c r="M24" s="1">
+        <v>38930479</v>
+      </c>
+      <c r="N24">
+        <v>25.71</v>
+      </c>
+      <c r="O24">
+        <v>0.41061636600000001</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="1"/>
+        <v>4.10616366</v>
+      </c>
+      <c r="R24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25">
+        <v>8192</v>
+      </c>
+      <c r="B25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25">
+        <v>32</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1360594186</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2047074514</v>
+      </c>
+      <c r="G25">
+        <v>1.5</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="I25" s="1">
+        <v>29484424</v>
+      </c>
+      <c r="J25" s="1">
+        <v>10419275</v>
+      </c>
+      <c r="K25">
+        <v>35.338000000000001</v>
+      </c>
+      <c r="L25" s="1">
+        <v>114908516</v>
+      </c>
+      <c r="M25" s="1">
+        <v>39806930</v>
+      </c>
+      <c r="N25">
+        <v>34.64</v>
+      </c>
+      <c r="O25">
+        <v>0.41590306999999999</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="1"/>
+        <v>4.1590306999999997</v>
+      </c>
+      <c r="R25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26">
+        <v>8192</v>
+      </c>
+      <c r="B26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26">
+        <v>32</v>
+      </c>
+      <c r="D26">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1603654501</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1857045450</v>
+      </c>
+      <c r="G26">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>115.99999999999999</v>
+      </c>
+      <c r="I26" s="1">
+        <v>39221576</v>
+      </c>
+      <c r="J26" s="1">
+        <v>8317148</v>
+      </c>
+      <c r="K26">
+        <v>21.206</v>
+      </c>
+      <c r="L26" s="1">
+        <v>100804701</v>
+      </c>
+      <c r="M26" s="1">
+        <v>55870990</v>
+      </c>
+      <c r="N26">
+        <v>55.42</v>
+      </c>
+      <c r="O26">
+        <v>0.489838459</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="1"/>
+        <v>4.89838459</v>
+      </c>
+      <c r="R26" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27">
+        <v>16384</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>10716881059</v>
+      </c>
+      <c r="F27" s="1">
+        <v>14719055674</v>
+      </c>
+      <c r="G27">
+        <v>1.37</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="I27" s="1">
+        <v>76884753</v>
+      </c>
+      <c r="J27" s="1">
+        <v>75330198</v>
+      </c>
+      <c r="K27">
+        <v>97.977999999999994</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1391419966</v>
+      </c>
+      <c r="M27" s="1">
+        <v>94792907</v>
+      </c>
+      <c r="N27">
+        <v>6.81</v>
+      </c>
+      <c r="O27">
+        <v>3.2381592719999999</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="1"/>
+        <v>32.38159272</v>
+      </c>
+      <c r="R27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28">
+        <v>16384</v>
+      </c>
+      <c r="B28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>8568651149</v>
+      </c>
+      <c r="F28" s="1">
+        <v>13783296790</v>
+      </c>
+      <c r="G28">
+        <v>1.61</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="I28" s="1">
+        <v>62152859</v>
+      </c>
+      <c r="J28" s="1">
+        <v>59496479</v>
+      </c>
+      <c r="K28">
+        <v>95.725999999999999</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1310878145</v>
+      </c>
+      <c r="M28" s="1">
+        <v>90395849</v>
+      </c>
+      <c r="N28">
+        <v>6.9</v>
+      </c>
+      <c r="O28">
+        <v>2.5908539230000001</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="1"/>
+        <v>25.908539230000002</v>
+      </c>
+      <c r="R28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29">
+        <v>16384</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29" s="1">
+        <v>6612925541</v>
+      </c>
+      <c r="F29" s="1">
+        <v>9964066457</v>
+      </c>
+      <c r="G29">
+        <v>1.51</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>151</v>
+      </c>
+      <c r="I29" s="1">
+        <v>63903627</v>
+      </c>
+      <c r="J29" s="1">
+        <v>60514689</v>
+      </c>
+      <c r="K29">
+        <v>94.697000000000003</v>
+      </c>
+      <c r="L29" s="1">
+        <v>618400669</v>
+      </c>
+      <c r="M29" s="1">
+        <v>93362475</v>
+      </c>
+      <c r="N29">
+        <v>15.1</v>
+      </c>
+      <c r="O29">
+        <v>1.9997543250000001</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>19.99754325</v>
+      </c>
+      <c r="R29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30">
+        <v>16384</v>
+      </c>
+      <c r="B30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>7795227177</v>
+      </c>
+      <c r="F30" s="1">
+        <v>13478233720</v>
+      </c>
+      <c r="G30">
+        <v>1.73</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>173</v>
+      </c>
+      <c r="I30" s="1">
+        <v>129939465</v>
+      </c>
+      <c r="J30" s="1">
+        <v>48842113</v>
+      </c>
+      <c r="K30">
+        <v>37.588000000000001</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1305454919</v>
+      </c>
+      <c r="M30" s="1">
+        <v>180473490</v>
+      </c>
+      <c r="N30">
+        <v>13.82</v>
+      </c>
+      <c r="O30">
+        <v>2.3575414220000002</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="1"/>
+        <v>23.575414220000003</v>
+      </c>
+      <c r="R30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31">
+        <v>16384</v>
+      </c>
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31">
+        <v>16</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1">
+        <v>5926844042</v>
+      </c>
+      <c r="F31" s="1">
+        <v>9797763595</v>
+      </c>
+      <c r="G31">
+        <v>1.65</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="I31" s="1">
+        <v>115835996</v>
+      </c>
+      <c r="J31" s="1">
+        <v>49491668</v>
+      </c>
+      <c r="K31">
+        <v>42.725999999999999</v>
+      </c>
+      <c r="L31" s="1">
+        <v>602357642</v>
+      </c>
+      <c r="M31" s="1">
+        <v>157973839</v>
+      </c>
+      <c r="N31">
+        <v>26.23</v>
+      </c>
+      <c r="O31">
+        <v>1.792620817</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>17.926208169999999</v>
+      </c>
+      <c r="R31" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32">
+        <v>16384</v>
+      </c>
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32">
+        <v>16</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1">
+        <v>5936802247</v>
+      </c>
+      <c r="F32" s="1">
+        <v>8162073083</v>
+      </c>
+      <c r="G32">
+        <v>1.37</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="I32" s="1">
+        <v>122796386</v>
+      </c>
+      <c r="J32" s="1">
+        <v>50221593</v>
+      </c>
+      <c r="K32">
+        <v>40.898000000000003</v>
+      </c>
+      <c r="L32" s="1">
+        <v>446122915</v>
+      </c>
+      <c r="M32" s="1">
+        <v>167766202</v>
+      </c>
+      <c r="N32">
+        <v>37.61</v>
+      </c>
+      <c r="O32">
+        <v>1.795718242</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="1"/>
+        <v>17.957182419999999</v>
+      </c>
+      <c r="R32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33">
+        <v>16384</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>7354726969</v>
+      </c>
+      <c r="F33" s="1">
+        <v>13367989963</v>
+      </c>
+      <c r="G33">
+        <v>1.82</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="I33" s="1">
+        <v>171365067</v>
+      </c>
+      <c r="J33" s="1">
+        <v>40873437</v>
+      </c>
+      <c r="K33">
+        <v>23.852</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1310947088</v>
+      </c>
+      <c r="M33" s="1">
+        <v>209512449</v>
+      </c>
+      <c r="N33">
+        <v>15.98</v>
+      </c>
+      <c r="O33">
+        <v>2.2237272219999999</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
+        <v>22.237272220000001</v>
+      </c>
+      <c r="R33" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34">
+        <v>16384</v>
+      </c>
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34">
+        <v>32</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34" s="1">
+        <v>5534287549</v>
+      </c>
+      <c r="F34" s="1">
+        <v>9757159093</v>
+      </c>
+      <c r="G34">
+        <v>1.76</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="I34" s="1">
+        <v>122204066</v>
+      </c>
+      <c r="J34" s="1">
+        <v>41813423</v>
+      </c>
+      <c r="K34">
+        <v>34.216000000000001</v>
+      </c>
+      <c r="L34" s="1">
+        <v>602921333</v>
+      </c>
+      <c r="M34" s="1">
+        <v>150248187</v>
+      </c>
+      <c r="N34">
+        <v>24.92</v>
+      </c>
+      <c r="O34">
+        <v>1.673177189</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="1"/>
+        <v>16.731771890000001</v>
+      </c>
+      <c r="R34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35">
+        <v>16384</v>
+      </c>
+      <c r="B35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35">
+        <v>32</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1">
+        <v>5500442448</v>
+      </c>
+      <c r="F35" s="1">
+        <v>8171883728</v>
+      </c>
+      <c r="G35">
+        <v>1.49</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="I35" s="1">
+        <v>117095123</v>
+      </c>
+      <c r="J35" s="1">
+        <v>41716902</v>
+      </c>
+      <c r="K35">
+        <v>35.627000000000002</v>
+      </c>
+      <c r="L35" s="1">
+        <v>456478893</v>
+      </c>
+      <c r="M35" s="1">
+        <v>158091097</v>
+      </c>
+      <c r="N35">
+        <v>34.630000000000003</v>
+      </c>
+      <c r="O35">
+        <v>1.6645724040000001</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="1"/>
+        <v>16.645724040000001</v>
+      </c>
+      <c r="R35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36">
+        <v>16384</v>
+      </c>
+      <c r="B36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36">
+        <v>32</v>
+      </c>
+      <c r="D36">
+        <v>16</v>
+      </c>
+      <c r="E36" s="1">
+        <v>6439999482</v>
+      </c>
+      <c r="F36" s="1">
+        <v>7410751715</v>
+      </c>
+      <c r="G36">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>114.99999999999999</v>
+      </c>
+      <c r="I36" s="1">
+        <v>157184193</v>
+      </c>
+      <c r="J36" s="1">
+        <v>33185775</v>
+      </c>
+      <c r="K36">
+        <v>21.113</v>
+      </c>
+      <c r="L36" s="1">
+        <v>401523831</v>
+      </c>
+      <c r="M36" s="1">
+        <v>223049879</v>
+      </c>
+      <c r="N36">
+        <v>55.55</v>
+      </c>
+      <c r="O36">
+        <v>1.947632783</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="1"/>
+        <v>19.476327829999999</v>
+      </c>
+      <c r="R36" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37">
+        <v>32768</v>
+      </c>
+      <c r="B37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>43354351943</v>
+      </c>
+      <c r="F37" s="1">
+        <v>58861589907</v>
+      </c>
+      <c r="G37">
+        <v>1.36</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="I37" s="1">
+        <v>307964080</v>
+      </c>
+      <c r="J37" s="1">
+        <v>300807132</v>
+      </c>
+      <c r="K37">
+        <v>97.676000000000002</v>
+      </c>
+      <c r="L37" s="1">
+        <v>5562028891</v>
+      </c>
+      <c r="M37" s="1">
+        <v>379952108</v>
+      </c>
+      <c r="N37">
+        <v>6.83</v>
+      </c>
+      <c r="O37">
+        <v>13.106439871999999</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="1"/>
+        <v>131.06439871999999</v>
+      </c>
+      <c r="R37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38">
+        <v>32768</v>
+      </c>
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1">
+        <v>34828792884</v>
+      </c>
+      <c r="F38" s="1">
+        <v>55123929251</v>
+      </c>
+      <c r="G38">
+        <v>1.58</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+      <c r="I38" s="1">
+        <v>249582163</v>
+      </c>
+      <c r="J38" s="1">
+        <v>238283738</v>
+      </c>
+      <c r="K38">
+        <v>95.472999999999999</v>
+      </c>
+      <c r="L38" s="1">
+        <v>5239845751</v>
+      </c>
+      <c r="M38" s="1">
+        <v>363839021</v>
+      </c>
+      <c r="N38">
+        <v>6.94</v>
+      </c>
+      <c r="O38">
+        <v>10.526721014</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="1"/>
+        <v>105.26721014</v>
+      </c>
+      <c r="R38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39">
+        <v>32768</v>
+      </c>
+      <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39" s="1">
+        <v>26141080558</v>
+      </c>
+      <c r="F39" s="1">
+        <v>39848852998</v>
+      </c>
+      <c r="G39">
+        <v>1.52</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="I39" s="1">
+        <v>254069989</v>
+      </c>
+      <c r="J39" s="1">
+        <v>240441962</v>
+      </c>
+      <c r="K39">
+        <v>94.635999999999996</v>
+      </c>
+      <c r="L39" s="1">
+        <v>2469817003</v>
+      </c>
+      <c r="M39" s="1">
+        <v>372039827</v>
+      </c>
+      <c r="N39">
+        <v>15.06</v>
+      </c>
+      <c r="O39">
+        <v>7.9009819380000001</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="1"/>
+        <v>79.009819379999996</v>
+      </c>
+      <c r="R39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40">
+        <v>32768</v>
+      </c>
+      <c r="B40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>31287844061</v>
+      </c>
+      <c r="F40" s="1">
+        <v>53904969292</v>
+      </c>
+      <c r="G40">
+        <v>1.72</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+      <c r="I40" s="1">
+        <v>519951824</v>
+      </c>
+      <c r="J40" s="1">
+        <v>195358320</v>
+      </c>
+      <c r="K40">
+        <v>37.572000000000003</v>
+      </c>
+      <c r="L40" s="1">
+        <v>5218402646</v>
+      </c>
+      <c r="M40" s="1">
+        <v>721692724</v>
+      </c>
+      <c r="N40">
+        <v>13.83</v>
+      </c>
+      <c r="O40">
+        <v>9.4540785639999996</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="1"/>
+        <v>94.540785639999996</v>
+      </c>
+      <c r="R40" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41">
+        <v>32768</v>
+      </c>
+      <c r="B41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41" s="1">
+        <v>23877820143</v>
+      </c>
+      <c r="F41" s="1">
+        <v>39184094375</v>
+      </c>
+      <c r="G41">
+        <v>1.64</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="I41" s="1">
+        <v>463698171</v>
+      </c>
+      <c r="J41" s="1">
+        <v>199368600</v>
+      </c>
+      <c r="K41">
+        <v>42.994999999999997</v>
+      </c>
+      <c r="L41" s="1">
+        <v>2405263423</v>
+      </c>
+      <c r="M41" s="1">
+        <v>631071808</v>
+      </c>
+      <c r="N41">
+        <v>26.24</v>
+      </c>
+      <c r="O41">
+        <v>7.2188005349999997</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="1"/>
+        <v>72.188005349999997</v>
+      </c>
+      <c r="R41" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42">
+        <v>32768</v>
+      </c>
+      <c r="B42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1">
+        <v>23886951896</v>
+      </c>
+      <c r="F42" s="1">
+        <v>32632875229</v>
+      </c>
+      <c r="G42">
+        <v>1.37</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="I42" s="1">
+        <v>491764569</v>
+      </c>
+      <c r="J42" s="1">
+        <v>201110887</v>
+      </c>
+      <c r="K42">
+        <v>40.896000000000001</v>
+      </c>
+      <c r="L42" s="1">
+        <v>1780835456</v>
+      </c>
+      <c r="M42" s="1">
+        <v>669532792</v>
+      </c>
+      <c r="N42">
+        <v>37.6</v>
+      </c>
+      <c r="O42">
+        <v>7.2226589920000004</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="1"/>
+        <v>72.226589920000009</v>
+      </c>
+      <c r="R42" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43">
+        <v>32768</v>
+      </c>
+      <c r="B43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43">
+        <v>32</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43" s="1">
+        <v>29587007952</v>
+      </c>
+      <c r="F43" s="1">
+        <v>53457406366</v>
+      </c>
+      <c r="G43">
+        <v>1.81</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+      <c r="I43" s="1">
+        <v>683967359</v>
+      </c>
+      <c r="J43" s="1">
+        <v>164131558</v>
+      </c>
+      <c r="K43">
+        <v>23.997</v>
+      </c>
+      <c r="L43" s="1">
+        <v>5241325834</v>
+      </c>
+      <c r="M43" s="1">
+        <v>835461353</v>
+      </c>
+      <c r="N43">
+        <v>15.94</v>
+      </c>
+      <c r="O43">
+        <v>8.941957961</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="1"/>
+        <v>89.41957961</v>
+      </c>
+      <c r="R43" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44">
+        <v>32768</v>
+      </c>
+      <c r="B44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44">
+        <v>32</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44" s="1">
+        <v>22293507761</v>
+      </c>
+      <c r="F44" s="1">
+        <v>39006729323</v>
+      </c>
+      <c r="G44">
+        <v>1.75</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="I44" s="1">
+        <v>489670647</v>
+      </c>
+      <c r="J44" s="1">
+        <v>168927573</v>
+      </c>
+      <c r="K44">
+        <v>34.497999999999998</v>
+      </c>
+      <c r="L44" s="1">
+        <v>2408094252</v>
+      </c>
+      <c r="M44" s="1">
+        <v>601629172</v>
+      </c>
+      <c r="N44">
+        <v>24.98</v>
+      </c>
+      <c r="O44">
+        <v>6.7492244030000004</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="1"/>
+        <v>67.492244030000009</v>
+      </c>
+      <c r="R44" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
+      <c r="A45">
+        <v>32768</v>
+      </c>
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45">
+        <v>32</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1">
+        <v>22500253191</v>
+      </c>
+      <c r="F45" s="1">
+        <v>32673395111</v>
+      </c>
+      <c r="G45">
+        <v>1.45</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="I45" s="1">
+        <v>470011087</v>
+      </c>
+      <c r="J45" s="1">
+        <v>170435618</v>
+      </c>
+      <c r="K45">
+        <v>36.262</v>
+      </c>
+      <c r="L45" s="1">
+        <v>1822928015</v>
+      </c>
+      <c r="M45" s="1">
+        <v>632334252</v>
+      </c>
+      <c r="N45">
+        <v>34.69</v>
+      </c>
+      <c r="O45">
+        <v>6.8043265760000002</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="1"/>
+        <v>68.043265759999997</v>
+      </c>
+      <c r="R45" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46">
+        <v>32768</v>
+      </c>
+      <c r="B46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46">
+        <v>32</v>
+      </c>
+      <c r="D46">
+        <v>16</v>
+      </c>
+      <c r="E46" s="1">
+        <v>27157187698</v>
+      </c>
+      <c r="F46" s="1">
+        <v>29648960880</v>
+      </c>
+      <c r="G46">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>109.00000000000001</v>
+      </c>
+      <c r="I46" s="1">
+        <v>644806896</v>
+      </c>
+      <c r="J46" s="1">
+        <v>130090567</v>
+      </c>
+      <c r="K46">
+        <v>20.175000000000001</v>
+      </c>
+      <c r="L46" s="1">
+        <v>1601071769</v>
+      </c>
+      <c r="M46" s="1">
+        <v>924913759</v>
+      </c>
+      <c r="N46">
+        <v>57.77</v>
+      </c>
+      <c r="O46">
+        <v>8.2088346219999995</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="1"/>
+        <v>82.088346219999991</v>
+      </c>
+      <c r="R46" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47">
+        <v>8192</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2209112525</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3191338468</v>
+      </c>
+      <c r="G47">
+        <v>1.44</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="I47" s="1">
+        <v>36832406</v>
+      </c>
+      <c r="J47" s="1">
+        <v>11754499</v>
+      </c>
+      <c r="K47">
+        <v>31.913</v>
+      </c>
+      <c r="L47" s="1">
+        <v>348584466</v>
+      </c>
+      <c r="M47" s="1">
+        <v>52851133</v>
+      </c>
+      <c r="N47">
+        <v>15.16</v>
+      </c>
+      <c r="O47">
+        <v>0.67644314800000005</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="1"/>
+        <v>6.7644314800000007</v>
+      </c>
+      <c r="R47" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48">
+        <v>16384</v>
+      </c>
+      <c r="B48" t="s">
+        <v>115</v>
+      </c>
+      <c r="E48" s="1">
+        <v>9188891718</v>
+      </c>
+      <c r="F48" s="1">
+        <v>12901535043</v>
+      </c>
+      <c r="G48">
+        <v>1.4</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="I48" s="1">
+        <v>144214273</v>
+      </c>
+      <c r="J48" s="1">
+        <v>60800617</v>
+      </c>
+      <c r="K48">
+        <v>42.16</v>
+      </c>
+      <c r="L48" s="1">
+        <v>1424218465</v>
+      </c>
+      <c r="M48" s="1">
+        <v>213663616</v>
+      </c>
+      <c r="N48">
+        <v>15</v>
+      </c>
+      <c r="O48">
+        <v>2.7805185099999998</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="1"/>
+        <v>27.805185099999999</v>
+      </c>
+      <c r="R48" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
+      <c r="A49">
+        <v>32768</v>
+      </c>
+      <c r="B49" t="s">
+        <v>115</v>
+      </c>
+      <c r="E49" s="1">
+        <v>40684762075</v>
+      </c>
+      <c r="F49" s="1">
+        <v>52136831127</v>
+      </c>
+      <c r="G49">
+        <v>1.28</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="I49" s="1">
+        <v>588905996</v>
+      </c>
+      <c r="J49" s="1">
+        <v>316146697</v>
+      </c>
+      <c r="K49">
+        <v>53.683999999999997</v>
+      </c>
+      <c r="L49" s="1">
+        <v>5828735532</v>
+      </c>
+      <c r="M49" s="1">
+        <v>890401918</v>
+      </c>
+      <c r="N49">
+        <v>15.28</v>
+      </c>
+      <c r="O49">
+        <v>12.29858684</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="1"/>
+        <v>122.9858684</v>
+      </c>
+      <c r="R49" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
+      <c r="A50">
+        <v>8192</v>
+      </c>
+      <c r="B50" t="s">
+        <v>196</v>
+      </c>
+      <c r="E50" s="1">
+        <v>2792551394</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1431383481</v>
+      </c>
+      <c r="G50">
+        <v>0.51</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="I50" s="1">
+        <v>59458321</v>
+      </c>
+      <c r="J50" s="1">
+        <v>39693623</v>
+      </c>
+      <c r="K50">
+        <v>66.759</v>
+      </c>
+      <c r="L50" s="1">
+        <v>72600476</v>
+      </c>
+      <c r="M50" s="1">
+        <v>64844818</v>
+      </c>
+      <c r="N50">
+        <v>89.32</v>
+      </c>
+      <c r="O50">
+        <v>0.85247108999999999</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="1"/>
+        <v>8.5247109000000005</v>
+      </c>
+      <c r="R50" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="A51">
+        <v>16384</v>
+      </c>
+      <c r="B51" t="s">
+        <v>196</v>
+      </c>
+      <c r="E51" s="1">
+        <v>11718137889</v>
+      </c>
+      <c r="F51" s="1">
+        <v>5706446347</v>
+      </c>
+      <c r="G51">
+        <v>0.49</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="I51" s="1">
+        <v>285463490</v>
+      </c>
+      <c r="J51" s="1">
+        <v>159511037</v>
+      </c>
+      <c r="K51">
+        <v>55.878</v>
+      </c>
+      <c r="L51" s="1">
+        <v>285164938</v>
+      </c>
+      <c r="M51" s="1">
+        <v>303909679</v>
+      </c>
+      <c r="N51">
+        <v>106.57</v>
+      </c>
+      <c r="O51">
+        <v>3.5420382610000001</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="1"/>
+        <v>35.420382610000004</v>
+      </c>
+      <c r="R51" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
+      <c r="A52">
+        <v>32768</v>
+      </c>
+      <c r="B52" t="s">
+        <v>196</v>
+      </c>
+      <c r="E52" s="1">
+        <v>68885579544</v>
+      </c>
+      <c r="F52" s="1">
+        <v>22832072767</v>
+      </c>
+      <c r="G52">
+        <v>0.33</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="I52" s="1">
+        <v>1542208615</v>
+      </c>
+      <c r="J52" s="1">
+        <v>680539307</v>
+      </c>
+      <c r="K52">
+        <v>44.128</v>
+      </c>
+      <c r="L52" s="1">
+        <v>1142152631</v>
+      </c>
+      <c r="M52" s="1">
+        <v>1628765633</v>
+      </c>
+      <c r="N52">
+        <v>142.6</v>
+      </c>
+      <c r="O52">
+        <v>20.807963248</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="1"/>
+        <v>208.07963247999999</v>
+      </c>
+      <c r="R52" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>